<commit_message>
rename the slac stat uncertainty so that the cj-format converting code can recognize it
</commit_message>
<xml_diff>
--- a/data/JAM/10010.xlsx
+++ b/data/JAM/10010.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="format" sheetId="1" state="visible" r:id="rId2"/>
@@ -64,13 +64,13 @@
     <t xml:space="preserve">value</t>
   </si>
   <si>
-    <t xml:space="preserve">stat</t>
+    <t xml:space="preserve">%ptp</t>
   </si>
   <si>
-    <t xml:space="preserve">syst</t>
+    <t xml:space="preserve">%sys</t>
   </si>
   <si>
-    <t xml:space="preserve">%dST_u</t>
+    <t xml:space="preserve">%stat_u</t>
   </si>
   <si>
     <t xml:space="preserve">%dSR_u</t>
@@ -288,15 +288,15 @@
   </sheetPr>
   <dimension ref="A1:AF664"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R6" activeCellId="0" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="8" min="1" style="1" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="13" min="9" style="2" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="1" width="12.0612244897959"/>
+    <col collapsed="false" hidden="false" max="13" min="9" style="2" width="12.5969387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="12.0612244897959"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
fix the end-of-file in slac_p
</commit_message>
<xml_diff>
--- a/data/JAM/10010.xlsx
+++ b/data/JAM/10010.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3338" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3337" uniqueCount="37">
   <si>
     <t xml:space="preserve">exp</t>
   </si>
@@ -131,9 +131,6 @@
   </si>
   <si>
     <t xml:space="preserve">NC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">file</t>
   </si>
 </sst>
 </file>
@@ -286,17 +283,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AF664"/>
+  <dimension ref="A1:AF662"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R6" activeCellId="0" sqref="R6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A650" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D668" activeCellId="0" sqref="D668"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="8" min="1" style="1" width="12.0612244897959"/>
-    <col collapsed="false" hidden="false" max="13" min="9" style="2" width="12.5969387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="12.0612244897959"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="1" width="12.5102040816327"/>
+    <col collapsed="false" hidden="false" max="13" min="9" style="2" width="13.0510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="12.5102040816327"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -65173,14 +65170,6 @@
       </c>
       <c r="AF662" s="1" t="n">
         <v>2.1</v>
-      </c>
-    </row>
-    <row r="663" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D663" s="0"/>
-    </row>
-    <row r="664" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D664" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>